<commit_message>
Working commit v1 12/12/14
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28220" yWindow="2200" windowWidth="23820" windowHeight="14940"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="Sub-Tasks" sheetId="3" r:id="rId4"/>
     <sheet name="Variables" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
   <si>
     <t>Project</t>
   </si>
@@ -43,21 +43,12 @@
     <t>Person</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>CAAR Web Site</t>
   </si>
   <si>
     <t>NCST Conference</t>
   </si>
   <si>
-    <t>ITS World Congress</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -254,13 +245,172 @@
   </si>
   <si>
     <t>Hardware</t>
+  </si>
+  <si>
+    <t>Tire Expo Booth 2015</t>
+  </si>
+  <si>
+    <t>Motocycle Summit 2015</t>
+  </si>
+  <si>
+    <t>File/Folder Clean-up</t>
+  </si>
+  <si>
+    <t>Subtask</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>News Release</t>
+  </si>
+  <si>
+    <t>Writing Content</t>
+  </si>
+  <si>
+    <t>Editing Content</t>
+  </si>
+  <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>E-Newsletter</t>
+  </si>
+  <si>
+    <t>Media Tracking</t>
+  </si>
+  <si>
+    <t>Ordering</t>
+  </si>
+  <si>
+    <t>Invoves writing for social media, news releases, for website, for blog posts, for conference and event materials</t>
+  </si>
+  <si>
+    <t>Communication Plan</t>
+  </si>
+  <si>
+    <t>Video Editing</t>
+  </si>
+  <si>
+    <t>Photo Editing</t>
+  </si>
+  <si>
+    <t>Head Shots</t>
+  </si>
+  <si>
+    <t>Marketing List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves filling out PAF and workign with fiscal team to get product/service from purchase to recieved stages </t>
+  </si>
+  <si>
+    <t>Involves examining researchers calendars</t>
+  </si>
+  <si>
+    <t>Coordinating Tours/Meetings/Events/Interviews</t>
+  </si>
+  <si>
+    <t>Media Contact</t>
+  </si>
+  <si>
+    <t>ICMPA9 2015</t>
+  </si>
+  <si>
+    <t>Creating Content</t>
+  </si>
+  <si>
+    <t>Involves creation of content by writing and may include some graphic manipulation,</t>
+  </si>
+  <si>
+    <t>MCOP Adaptive Lighting Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional Development -Training </t>
+  </si>
+  <si>
+    <t>Updating Invitation List</t>
+  </si>
+  <si>
+    <t>Involves moifying or editing existing content such as news releases, web content, blog posts, and  graphic materials</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves vetting candidates for employement or internships. Can involve resume review, interviews, and any paperwor/training involved to support new team memeber. </t>
+  </si>
+  <si>
+    <t>Sharing Video/Graphics with Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves a variety of tasks associated with hiring new employees/interns/ supervisory tasks such as signing time sheets and conducting performance evaluations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves taking media calls/emails and answering questions. Can also invlve connecting member of the media with various researchers and setting up site visits. </t>
+  </si>
+  <si>
+    <t>Involves the coordination of the ICMPA9 conference being hosted in May 2015.</t>
+  </si>
+  <si>
+    <t>Involves the creation,editing and updating the UTC Website</t>
+  </si>
+  <si>
+    <t>Involves</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Completed project</t>
+  </si>
+  <si>
+    <t>Involved the writting of the RFP for the NCST Conference - complete</t>
+  </si>
+  <si>
+    <t>Involves the content management and periodic update for the VTTI Intranet page.</t>
+  </si>
+  <si>
+    <t>Involves the event planing, graphic developments and logistical coordination for the SAE 2015 GIM meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the logistical coordination of </t>
+  </si>
+  <si>
+    <t>Reporting  - git hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the reporting of time spent on various projects and mantanace of sotware on personal computers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the creation, editing and approval process associated with the development delivery of the VTTI annual report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the collaboration with the GCAPS team to execute graphics, videos, advertisements and content for the annual Tire Expo the team attends. </t>
+  </si>
+  <si>
+    <t>Involves the creation, editing and distribution of AVS One Pagers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the management and </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the management, frequesnt updates and backups of the VTTI website. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves providing support to the AVS/NSTSCE Team for recording of videos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves the coordination, graphics development and logistical </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,16 +418,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -285,11 +470,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,8 +507,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -472,7 +684,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -850,7 +1062,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -858,11 +1070,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -883,10 +1095,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -897,13 +1109,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -912,18 +1124,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>2014</v>
@@ -932,18 +1144,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>2014</v>
@@ -952,18 +1164,18 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>2014</v>
@@ -972,18 +1184,18 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>2014</v>
@@ -992,18 +1204,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -1012,18 +1224,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>2014</v>
@@ -1032,18 +1244,18 @@
         <v>1.25</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>2014</v>
@@ -1052,18 +1264,18 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>2014</v>
@@ -1072,18 +1284,18 @@
         <v>1.75</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>2014</v>
@@ -1092,18 +1304,18 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>2014</v>
@@ -1112,18 +1324,18 @@
         <v>6.5</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>2014</v>
@@ -1132,18 +1344,18 @@
         <v>1.25</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1152,18 +1364,18 @@
         <v>0.75</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1172,18 +1384,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>2014</v>
@@ -1192,18 +1404,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>2014</v>
@@ -1212,18 +1424,18 @@
         <v>4.5</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>2014</v>
@@ -1232,18 +1444,18 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>2014</v>
@@ -1252,18 +1464,18 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>2014</v>
@@ -1272,18 +1484,18 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>2014</v>
@@ -1292,18 +1504,18 @@
         <v>1.5</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>2014</v>
@@ -1312,18 +1524,18 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>2014</v>
@@ -1332,18 +1544,18 @@
         <v>3.5</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24">
         <v>2014</v>
@@ -1352,18 +1564,18 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>2014</v>
@@ -1372,18 +1584,18 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>2014</v>
@@ -1392,18 +1604,18 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>2014</v>
@@ -1412,18 +1624,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <v>2014</v>
@@ -1432,18 +1644,18 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>2014</v>
@@ -1452,18 +1664,18 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>2014</v>
@@ -1472,18 +1684,18 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>2014</v>
@@ -1492,18 +1704,18 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>2014</v>
@@ -1512,18 +1724,18 @@
         <v>0.5</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>2014</v>
@@ -1532,12 +1744,67 @@
         <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34">
+        <v>2014</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>2014</v>
+      </c>
+      <c r="E35" s="5">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>2014</v>
+      </c>
+      <c r="E36" s="5">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1554,12 +1821,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Project List'!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>A1:A1048573</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Variables!$A:$A</xm:f>
@@ -1584,6 +1845,12 @@
           </x14:formula1>
           <xm:sqref>B2:B1048573</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Project List'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048573</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1598,7 +1865,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1609,10 +1876,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1620,20 +1887,20 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>7</v>
@@ -1641,7 +1908,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
         <v>7</v>
@@ -1649,7 +1916,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>7</v>
@@ -1657,7 +1924,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
@@ -1665,7 +1932,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -1673,7 +1940,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -1681,7 +1948,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
@@ -1689,7 +1956,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -1697,7 +1964,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -1705,7 +1972,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
         <v>17</v>
@@ -1729,117 +1996,235 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="122.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>54</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>60</v>
       </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1850,140 +2235,222 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" customWidth="1"/>
+    <col min="2" max="2" width="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>74</v>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2001,17 +2468,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1">
         <v>2014</v>
@@ -2019,10 +2486,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>2015</v>
@@ -2030,10 +2497,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>2016</v>
@@ -2041,10 +2508,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2017</v>
@@ -2052,10 +2519,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -2063,21 +2530,18 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>2019</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2020</v>
@@ -2085,7 +2549,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -2093,7 +2557,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>2022</v>
@@ -2101,7 +2565,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>2023</v>
@@ -2109,12 +2573,12 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12.5.14 - Ceci Hours
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="149">
   <si>
     <t>Project</t>
   </si>
@@ -597,13 +597,13 @@
   <dxfs count="3">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -760,7 +760,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -852,10 +852,10 @@
     <dataField name="Sum of Hours" fld="4" baseField="0" baseItem="1566352" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -876,7 +876,7 @@
     <tableColumn id="2" name="Sub-Task"/>
     <tableColumn id="6" name="Month"/>
     <tableColumn id="7" name="Year"/>
-    <tableColumn id="4" name="Hours" dataDxfId="0"/>
+    <tableColumn id="4" name="Hours" dataDxfId="2"/>
     <tableColumn id="5" name="Person"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1138,7 +1138,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1146,11 +1146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2060,6 +2060,26 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46">
+        <v>2014</v>
+      </c>
+      <c r="E46" s="5">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2120,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D45" sqref="D45:D46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added subtask descriptions - justin 12/12/14
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vtti.ad.vt.edu\data\Users\jfine\private\Desktop\GitHub\timesheet\Spreadsheet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31540" yWindow="0" windowWidth="28800" windowHeight="17560" activeTab="3"/>
+    <workbookView xWindow="-31545" yWindow="0" windowWidth="28800" windowHeight="17565" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -15,21 +20,21 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="165">
   <si>
     <t>Project</t>
   </si>
@@ -418,9 +423,6 @@
     <t>Coordination</t>
   </si>
   <si>
-    <t>Involves manipulating a photo to improve the look. Is provided upon request.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Involves signing up and attending various trainings either mandatory or for professional development. </t>
   </si>
   <si>
@@ -433,9 +435,6 @@
     <t xml:space="preserve">Involves creating, editing, emailing, printing and delivering of various event/conference invitations. </t>
   </si>
   <si>
-    <t xml:space="preserve">Involves live filming and prep time for recording videos. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Involves assisting center directors/group leaders in RFP delivery to win event or conference bid. </t>
   </si>
   <si>
@@ -463,12 +462,6 @@
     <t xml:space="preserve">Involves filling out PAF and working with fiscal team to get product/service from purchase to received stages </t>
   </si>
   <si>
-    <t>Video editing</t>
-  </si>
-  <si>
-    <t>Photo editing</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRMO Team focused meetings, brainstorming, management, collaborations. </t>
   </si>
   <si>
@@ -476,6 +469,66 @@
   </si>
   <si>
     <t>Involves attendance  and coordination for Tours/Meetings/Events/Interviews/Demos. May involve attending meetings, examining researchers calendars, sending emails, submitting necessary forms and answering phone calls to setup activity.</t>
+  </si>
+  <si>
+    <t>Involves editing, revising, incorporating feedback into a small scale/size graphic</t>
+  </si>
+  <si>
+    <t>Involves editing, revising, incorporating feedback into a moderate scale/size graphic</t>
+  </si>
+  <si>
+    <t>Involves editing, revising, incorporating feedback into a large scale/size graphic</t>
+  </si>
+  <si>
+    <t>Small graphic creation</t>
+  </si>
+  <si>
+    <t>Involves researching/gathering information, ideation and production of a small scale/size graphic</t>
+  </si>
+  <si>
+    <t>Involves researching/gathering information, ideation and production of a moderate scale/size graphic</t>
+  </si>
+  <si>
+    <t>Involves researching/gathering information, ideation and production of a large scale/size graphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves actually setting graphic components into motion and cultivating weight, feel and timing </t>
+  </si>
+  <si>
+    <t>Photography - Preproduction</t>
+  </si>
+  <si>
+    <t>Involves planning the photoshoot: gathering necessary materials and personnel.</t>
+  </si>
+  <si>
+    <t>Photography - Production</t>
+  </si>
+  <si>
+    <t>Involves executing the photoshoot</t>
+  </si>
+  <si>
+    <t>Photography - Postproduction</t>
+  </si>
+  <si>
+    <t>Involves file upload, color correction, exposure balancing, general digital touch-ups</t>
+  </si>
+  <si>
+    <t>Involves cleaning up files and reorganizing the workspace</t>
+  </si>
+  <si>
+    <t>Video - Preproduction</t>
+  </si>
+  <si>
+    <t>Involves planning principal photography, scheduling, gathering materials and storyboarding</t>
+  </si>
+  <si>
+    <t>Video - Production</t>
+  </si>
+  <si>
+    <t>Involves executing principal photography and audio</t>
+  </si>
+  <si>
+    <t>Video - Postproduction</t>
   </si>
 </sst>
 </file>
@@ -515,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,7 +621,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -576,6 +635,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -753,7 +813,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -1131,7 +1191,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1146,17 +1206,17 @@
       <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1196,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1236,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1276,7 +1336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1296,7 +1356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1316,7 +1376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1336,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1356,7 +1416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1376,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1416,7 +1476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1436,7 +1496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1456,7 +1516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1476,7 +1536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1496,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1516,7 +1576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1536,7 +1596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1556,12 +1616,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
@@ -1576,7 +1636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1596,7 +1656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1616,7 +1676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1636,7 +1696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1656,7 +1716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1676,7 +1736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1696,7 +1756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1716,12 +1776,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
@@ -1736,7 +1796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1756,7 +1816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1776,7 +1836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1796,7 +1856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1816,7 +1876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1836,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -1856,7 +1916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -1876,7 +1936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1896,9 +1956,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
         <v>128</v>
@@ -1916,7 +1976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1936,7 +1996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1956,7 +2016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1976,7 +2036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1996,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2016,7 +2076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -2036,7 +2096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -2056,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -2137,13 +2197,13 @@
       <selection activeCell="D45" sqref="D45:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2151,7 +2211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2159,7 +2219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2167,7 +2227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2183,7 +2243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2191,7 +2251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2199,7 +2259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2207,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -2223,7 +2283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2231,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -2239,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -2247,10 +2307,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16"/>
     </row>
   </sheetData>
@@ -2271,14 +2331,14 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="122.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="122.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickTop="1" thickBot="1">
+    <row r="1" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2297,12 +2357,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2310,7 +2370,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2318,7 +2378,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2326,7 +2386,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2334,7 +2394,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -2342,12 +2402,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2355,7 +2415,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2363,7 +2423,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2371,12 +2431,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2384,7 +2444,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2392,12 +2452,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -2405,7 +2465,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -2413,7 +2473,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -2421,7 +2481,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -2429,7 +2489,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2437,7 +2497,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2445,7 +2505,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -2453,7 +2513,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2461,7 +2521,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2469,7 +2529,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2477,7 +2537,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2485,7 +2545,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -2493,7 +2553,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2501,7 +2561,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2509,15 +2569,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>113</v>
       </c>
@@ -2538,19 +2598,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" customWidth="1"/>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
     <col min="2" max="2" width="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -2558,7 +2618,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -2566,220 +2626,273 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="B15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2800,9 +2913,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2813,7 +2926,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2824,7 +2937,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2835,7 +2948,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2846,7 +2959,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2857,7 +2970,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2868,7 +2981,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -2876,7 +2989,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -2884,7 +2997,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -2892,7 +3005,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -2900,12 +3013,12 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
12/12/14 hours update/descriptions added
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vtti.ad.vt.edu\data\Users\jfine\private\Desktop\GitHub\timesheet\Spreadsheet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31545" yWindow="0" windowWidth="28800" windowHeight="17565" activeTab="3"/>
+    <workbookView xWindow="-31545" yWindow="0" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="171">
   <si>
     <t>Project</t>
   </si>
@@ -529,6 +524,24 @@
   </si>
   <si>
     <t>Video - Postproduction</t>
+  </si>
+  <si>
+    <t>Communication regarding the task at hand</t>
+  </si>
+  <si>
+    <t>Answering general questions not related to any projects</t>
+  </si>
+  <si>
+    <t>Making sure the TRB demo site is live, functioning and accessible to those who need it</t>
+  </si>
+  <si>
+    <t>Maintaining the hardware (mostly the computers for LCD panels), making sure they're updating and not displaying errors</t>
+  </si>
+  <si>
+    <t>University required training</t>
+  </si>
+  <si>
+    <t>Going through the motions of getting Ensemble to do what I need it to do for various projects</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1204,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1199,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1497,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1550,7 +1563,7 @@
         <v>2014</v>
       </c>
       <c r="E17" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -1570,7 +1583,7 @@
         <v>2014</v>
       </c>
       <c r="E18" s="5">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -1610,7 +1623,7 @@
         <v>2014</v>
       </c>
       <c r="E20" s="5">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -2134,6 +2147,46 @@
       </c>
       <c r="F46" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47">
+        <v>2014</v>
+      </c>
+      <c r="E47" s="5">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48">
+        <v>2014</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2600,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,6 +2810,9 @@
       <c r="A20" t="s">
         <v>122</v>
       </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2778,11 +2834,17 @@
       <c r="A23" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>58</v>
       </c>
+      <c r="B24" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2796,15 +2858,24 @@
       <c r="A26" s="7" t="s">
         <v>124</v>
       </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Test Refresh Box"
This reverts commit 5cb67299f415a1e6ea4bc398e50f6969a5789505.
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565" activeTab="1"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="140001" refMode="R1C1"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
   <si>
     <t>Project</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Person</t>
   </si>
   <si>
+    <t>CAAR Web Site</t>
+  </si>
+  <si>
     <t>NCST Conference</t>
   </si>
   <si>
@@ -157,6 +160,9 @@
   </si>
   <si>
     <t>Invitations</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
   </si>
   <si>
     <t>Git Hub</t>
@@ -517,19 +523,7 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -554,63 +548,27 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Roderick Hall" refreshedDate="41989.420626736108" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="36">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Cecilia Elpi" refreshedDate="41975.701138773147" createdVersion="5" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Work Database"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Project" numFmtId="0">
-      <sharedItems containsBlank="1" count="21">
+      <sharedItems containsBlank="1" count="5">
         <s v="NCST Conference"/>
+        <s v="CAAR Web Site"/>
         <s v="NDRS Conference 2016"/>
-        <s v="Git Hub"/>
         <s v="TRB 2015"/>
-        <s v="SAE 2015 BrainCloud video"/>
-        <s v="Tire Expo Booth"/>
-        <s v="Annual Report"/>
-        <s v="Misc"/>
-        <s v="UTC Web Site"/>
-        <s v="AVS One-Pagers"/>
-        <s v="Intranet"/>
-        <s v="VTTI Redesign"/>
-        <s v="Employee Directory"/>
-        <s v="VTTI Website"/>
-        <s v="NSTSCE Video"/>
-        <s v="LCD Panels"/>
-        <s v="ICMPA9 2015"/>
-        <s v="Motocycle Summit 2015"/>
-        <s v="MCOP Adaptive Lighting Project"/>
         <m/>
-        <s v="CAAR Web Site" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Sub-Task" numFmtId="0">
-      <sharedItems containsBlank="1" count="25">
+      <sharedItems containsBlank="1" count="5">
         <s v="RFP Submission"/>
+        <s v="Update"/>
         <s v="Conference Planning"/>
-        <s v="Set up &amp; Instruction"/>
-        <s v="Large Graphic Edit"/>
-        <s v="Medium graphic creation"/>
-        <s v="Animation"/>
-        <s v="Large graphic creation"/>
-        <s v="Small Graphic Edit"/>
-        <s v="Photography"/>
-        <s v="Update"/>
-        <s v="Creation"/>
-        <s v="Dealing with Ensemble"/>
-        <s v="File Clean-up"/>
-        <s v="Printing"/>
-        <s v="Filming"/>
-        <s v="Communication"/>
-        <s v="Training"/>
-        <s v="Answering Questions"/>
-        <s v="Demo Site"/>
-        <s v="Hardware"/>
-        <s v="Editing Content"/>
-        <s v="Creating Content"/>
-        <s v="Writing Content"/>
+        <s v="Invitations"/>
         <m/>
-        <s v="Invitations" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Month" numFmtId="0">
@@ -624,15 +582,15 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2014"/>
     </cacheField>
     <cacheField name="Hours" numFmtId="2">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="8"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="Person" numFmtId="0">
       <sharedItems containsBlank="1" count="6">
         <s v="Rodd"/>
+        <s v="April"/>
         <s v="Ceci"/>
         <s v="Marin"/>
         <s v="Justin"/>
-        <s v="April"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -646,7 +604,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="36">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -657,11 +615,19 @@
   </r>
   <r>
     <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -669,11 +635,19 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="4"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
@@ -685,7 +659,7 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -693,243 +667,19 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.25"/>
-    <x v="3"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2014"/>
-    <n v="0.5"/>
-    <x v="3"/>
+    <n v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="4"/>
     <x v="4"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.75"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="5"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="6"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="6.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="7"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.25"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="8"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.75"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="10"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="10"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="6"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="11"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="12"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="13"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="14"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="14"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="15"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="2"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="15"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="16"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="17"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="19"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="20"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <x v="21"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="22"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="23"/>
     <x v="2"/>
     <m/>
     <m/>
@@ -939,68 +689,32 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item m="1" x="20"/>
+      <items count="6">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="19"/>
-        <item x="2"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="26">
-        <item x="1"/>
-        <item m="1" x="24"/>
-        <item x="0"/>
-        <item x="9"/>
-        <item x="23"/>
+      <items count="6">
         <item x="2"/>
         <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item h="1" x="2"/>
         <item t="default"/>
@@ -1010,10 +724,10 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="7">
+        <item x="1"/>
+        <item x="2"/>
         <item x="4"/>
-        <item x="1"/>
         <item x="3"/>
-        <item x="2"/>
         <item x="0"/>
         <item x="5"/>
         <item t="default"/>
@@ -1024,132 +738,33 @@
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="43">
+  <rowItems count="10">
     <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="10"/>
+      <x/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="1"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="12"/>
+      <x v="2"/>
     </i>
     <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1166,10 +781,10 @@
     <dataField name="Sum of Hours" fld="4" baseField="0" baseItem="1566352" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -1190,7 +805,7 @@
     <tableColumn id="2" name="Sub-Task"/>
     <tableColumn id="6" name="Month"/>
     <tableColumn id="7" name="Year"/>
-    <tableColumn id="4" name="Hours" dataDxfId="6"/>
+    <tableColumn id="4" name="Hours" dataDxfId="2"/>
     <tableColumn id="5" name="Person"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1462,9 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,10 +1100,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1499,13 +1114,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -1514,18 +1129,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>2014</v>
@@ -1534,18 +1149,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>2014</v>
@@ -1554,18 +1169,18 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>2014</v>
@@ -1574,18 +1189,18 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>2014</v>
@@ -1594,18 +1209,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -1614,18 +1229,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>2014</v>
@@ -1634,18 +1249,18 @@
         <v>1.25</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>2014</v>
@@ -1654,18 +1269,18 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>2014</v>
@@ -1674,18 +1289,18 @@
         <v>1.75</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>2014</v>
@@ -1694,18 +1309,18 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>2014</v>
@@ -1714,18 +1329,18 @@
         <v>6.5</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>2014</v>
@@ -1734,18 +1349,18 @@
         <v>1.25</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1754,18 +1369,18 @@
         <v>0.75</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1774,18 +1389,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>2014</v>
@@ -1794,18 +1409,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>2014</v>
@@ -1814,18 +1429,18 @@
         <v>4.5</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>2014</v>
@@ -1834,18 +1449,18 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>2014</v>
@@ -1854,18 +1469,18 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>2014</v>
@@ -1874,18 +1489,18 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>2014</v>
@@ -1894,18 +1509,18 @@
         <v>1.5</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>2014</v>
@@ -1914,18 +1529,18 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>2014</v>
@@ -1934,18 +1549,18 @@
         <v>3.5</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24">
         <v>2014</v>
@@ -1954,18 +1569,18 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>2014</v>
@@ -1974,18 +1589,18 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>2014</v>
@@ -1994,18 +1609,18 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>2014</v>
@@ -2014,18 +1629,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <v>2014</v>
@@ -2034,18 +1649,18 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>2014</v>
@@ -2054,18 +1669,18 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>2014</v>
@@ -2074,18 +1689,18 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>2014</v>
@@ -2094,18 +1709,18 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>2014</v>
@@ -2114,18 +1729,18 @@
         <v>0.5</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>2014</v>
@@ -2134,18 +1749,18 @@
         <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>2014</v>
@@ -2154,18 +1769,18 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>2014</v>
@@ -2174,18 +1789,18 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D36">
         <v>2014</v>
@@ -2194,7 +1809,7 @@
         <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2252,24 +1867,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,378 +1892,102 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>1.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
-        <v>1.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
-        <v>4.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4">
-        <v>1.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
-        <v>1.25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1.25</v>
-      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="4">
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="4">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="4">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="4">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53"/>
+      <c r="B16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2680,212 +2019,212 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2915,208 +2254,208 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
         <v>103</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +2480,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1">
         <v>2014</v>
@@ -3152,10 +2491,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>2015</v>
@@ -3163,10 +2502,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>2016</v>
@@ -3174,10 +2513,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2017</v>
@@ -3185,10 +2524,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -3196,10 +2535,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>2019</v>
@@ -3207,7 +2546,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2020</v>
@@ -3215,7 +2554,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -3223,7 +2562,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>2022</v>
@@ -3231,7 +2570,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>2023</v>
@@ -3239,12 +2578,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Test Refresh Box""
This reverts commit 630ab6a7f26df04177cd4550a31d245471aa052f.
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="140001" refMode="R1C1"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="21" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="123">
   <si>
     <t>Project</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Person</t>
   </si>
   <si>
-    <t>CAAR Web Site</t>
-  </si>
-  <si>
     <t>NCST Conference</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>Invitations</t>
-  </si>
-  <si>
-    <t>(Multiple Items)</t>
   </si>
   <si>
     <t>Git Hub</t>
@@ -523,7 +517,19 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -548,27 +554,63 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Cecilia Elpi" refreshedDate="41975.701138773147" createdVersion="5" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Roderick Hall" refreshedDate="41989.420626736108" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="36">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Work Database"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Project" numFmtId="0">
-      <sharedItems containsBlank="1" count="5">
+      <sharedItems containsBlank="1" count="21">
         <s v="NCST Conference"/>
-        <s v="CAAR Web Site"/>
         <s v="NDRS Conference 2016"/>
+        <s v="Git Hub"/>
         <s v="TRB 2015"/>
+        <s v="SAE 2015 BrainCloud video"/>
+        <s v="Tire Expo Booth"/>
+        <s v="Annual Report"/>
+        <s v="Misc"/>
+        <s v="UTC Web Site"/>
+        <s v="AVS One-Pagers"/>
+        <s v="Intranet"/>
+        <s v="VTTI Redesign"/>
+        <s v="Employee Directory"/>
+        <s v="VTTI Website"/>
+        <s v="NSTSCE Video"/>
+        <s v="LCD Panels"/>
+        <s v="ICMPA9 2015"/>
+        <s v="Motocycle Summit 2015"/>
+        <s v="MCOP Adaptive Lighting Project"/>
         <m/>
+        <s v="CAAR Web Site" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Sub-Task" numFmtId="0">
-      <sharedItems containsBlank="1" count="5">
+      <sharedItems containsBlank="1" count="25">
         <s v="RFP Submission"/>
+        <s v="Conference Planning"/>
+        <s v="Set up &amp; Instruction"/>
+        <s v="Large Graphic Edit"/>
+        <s v="Medium graphic creation"/>
+        <s v="Animation"/>
+        <s v="Large graphic creation"/>
+        <s v="Small Graphic Edit"/>
+        <s v="Photography"/>
         <s v="Update"/>
-        <s v="Conference Planning"/>
-        <s v="Invitations"/>
+        <s v="Creation"/>
+        <s v="Dealing with Ensemble"/>
+        <s v="File Clean-up"/>
+        <s v="Printing"/>
+        <s v="Filming"/>
+        <s v="Communication"/>
+        <s v="Training"/>
+        <s v="Answering Questions"/>
+        <s v="Demo Site"/>
+        <s v="Hardware"/>
+        <s v="Editing Content"/>
+        <s v="Creating Content"/>
+        <s v="Writing Content"/>
         <m/>
+        <s v="Invitations" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Month" numFmtId="0">
@@ -582,15 +624,15 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2014"/>
     </cacheField>
     <cacheField name="Hours" numFmtId="2">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="8"/>
     </cacheField>
     <cacheField name="Person" numFmtId="0">
       <sharedItems containsBlank="1" count="6">
         <s v="Rodd"/>
-        <s v="April"/>
         <s v="Ceci"/>
         <s v="Marin"/>
         <s v="Justin"/>
+        <s v="April"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -604,7 +646,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="36">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -615,19 +657,11 @@
   </r>
   <r>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -635,19 +669,11 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="4"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="5"/>
-    <x v="1"/>
-  </r>
-  <r>
     <x v="2"/>
-    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
@@ -659,7 +685,7 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -667,19 +693,243 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1.25"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2014"/>
-    <n v="1"/>
-    <x v="2"/>
+    <n v="0.5"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
     <x v="4"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1.75"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="6.5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1.25"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="0.75"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="4.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="12"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="13"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="3.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="15"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="15"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="16"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="17"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="0.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="0.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="19"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="0.5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="20"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="21"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="22"/>
+    <x v="1"/>
+    <n v="2014"/>
+    <n v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="23"/>
     <x v="2"/>
     <m/>
     <m/>
@@ -689,32 +939,68 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="22">
+        <item m="1" x="20"/>
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
+        <item x="3"/>
+        <item x="19"/>
         <item x="2"/>
-        <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="26">
+        <item x="1"/>
+        <item m="1" x="24"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="23"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
         <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item x="1"/>
         <item h="1" x="2"/>
         <item t="default"/>
@@ -724,10 +1010,10 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="7">
+        <item x="4"/>
         <item x="1"/>
+        <item x="3"/>
         <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
         <item x="0"/>
         <item x="5"/>
         <item t="default"/>
@@ -738,33 +1024,132 @@
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="43">
     <i>
-      <x/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="11"/>
     </i>
     <i r="1">
-      <x v="2"/>
+      <x v="12"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="12"/>
     </i>
     <i r="1">
-      <x/>
+      <x v="3"/>
     </i>
     <i r="1">
-      <x v="2"/>
+      <x v="17"/>
     </i>
     <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
       <x v="3"/>
     </i>
+    <i>
+      <x v="15"/>
+    </i>
     <i r="1">
-      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
     </i>
     <i t="grand">
       <x/>
@@ -781,10 +1166,10 @@
     <dataField name="Sum of Hours" fld="4" baseField="0" baseItem="1566352" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -805,7 +1190,7 @@
     <tableColumn id="2" name="Sub-Task"/>
     <tableColumn id="6" name="Month"/>
     <tableColumn id="7" name="Year"/>
-    <tableColumn id="4" name="Hours" dataDxfId="2"/>
+    <tableColumn id="4" name="Hours" dataDxfId="6"/>
     <tableColumn id="5" name="Person"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1077,9 +1462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1485,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1114,13 +1499,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -1129,18 +1514,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>2014</v>
@@ -1149,18 +1534,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>2014</v>
@@ -1169,18 +1554,18 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>2014</v>
@@ -1189,18 +1574,18 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>2014</v>
@@ -1209,18 +1594,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -1229,18 +1614,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>2014</v>
@@ -1249,18 +1634,18 @@
         <v>1.25</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>2014</v>
@@ -1269,18 +1654,18 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>2014</v>
@@ -1289,18 +1674,18 @@
         <v>1.75</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>2014</v>
@@ -1309,18 +1694,18 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>2014</v>
@@ -1329,18 +1714,18 @@
         <v>6.5</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>2014</v>
@@ -1349,18 +1734,18 @@
         <v>1.25</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1369,18 +1754,18 @@
         <v>0.75</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1389,18 +1774,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>2014</v>
@@ -1409,18 +1794,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>2014</v>
@@ -1429,18 +1814,18 @@
         <v>4.5</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18">
         <v>2014</v>
@@ -1449,18 +1834,18 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>2014</v>
@@ -1469,18 +1854,18 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>2014</v>
@@ -1489,18 +1874,18 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>2014</v>
@@ -1509,18 +1894,18 @@
         <v>1.5</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>2014</v>
@@ -1529,18 +1914,18 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23">
         <v>2014</v>
@@ -1549,18 +1934,18 @@
         <v>3.5</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>2014</v>
@@ -1569,18 +1954,18 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>2014</v>
@@ -1589,18 +1974,18 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26">
         <v>2014</v>
@@ -1609,18 +1994,18 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27">
         <v>2014</v>
@@ -1629,18 +2014,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28">
         <v>2014</v>
@@ -1649,18 +2034,18 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29">
         <v>2014</v>
@@ -1669,18 +2054,18 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30">
         <v>2014</v>
@@ -1689,18 +2074,18 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31">
         <v>2014</v>
@@ -1709,18 +2094,18 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32">
         <v>2014</v>
@@ -1729,18 +2114,18 @@
         <v>0.5</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33">
         <v>2014</v>
@@ -1749,18 +2134,18 @@
         <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>2014</v>
@@ -1769,18 +2154,18 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35">
         <v>2014</v>
@@ -1789,18 +2174,18 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36">
         <v>2014</v>
@@ -1809,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1867,24 +2252,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1892,102 +2277,378 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4">
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4">
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4">
-        <v>7</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4">
-        <v>7</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4">
-        <v>2</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4">
-        <v>1</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4">
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4">
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4">
-        <v>17</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15"/>
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16"/>
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2019,212 +2680,212 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2254,208 +2915,208 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2480,10 +3141,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1">
         <v>2014</v>
@@ -2491,10 +3152,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>2015</v>
@@ -2502,10 +3163,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>2016</v>
@@ -2513,10 +3174,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2017</v>
@@ -2524,10 +3185,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -2535,10 +3196,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>2019</v>
@@ -2546,7 +3207,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>2020</v>
@@ -2554,7 +3215,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -2562,7 +3223,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>2022</v>
@@ -2570,7 +3231,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>2023</v>
@@ -2578,12 +3239,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Test Refresh Box"""
This reverts commit fc2fd17ea2374b95519ec14448643de170eb4587.
</commit_message>
<xml_diff>
--- a/Project Documentation.xlsx
+++ b/Project Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565" activeTab="1"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="20565"/>
   </bookViews>
   <sheets>
     <sheet name="Work Database" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="140001" refMode="R1C1"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
   <si>
     <t>Project</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Person</t>
   </si>
   <si>
+    <t>CAAR Web Site</t>
+  </si>
+  <si>
     <t>NCST Conference</t>
   </si>
   <si>
@@ -157,6 +160,9 @@
   </si>
   <si>
     <t>Invitations</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
   </si>
   <si>
     <t>Git Hub</t>
@@ -517,19 +523,7 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -554,63 +548,27 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Roderick Hall" refreshedDate="41989.420626736108" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="36">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Cecilia Elpi" refreshedDate="41975.701138773147" createdVersion="5" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Work Database"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Project" numFmtId="0">
-      <sharedItems containsBlank="1" count="21">
+      <sharedItems containsBlank="1" count="5">
         <s v="NCST Conference"/>
+        <s v="CAAR Web Site"/>
         <s v="NDRS Conference 2016"/>
-        <s v="Git Hub"/>
         <s v="TRB 2015"/>
-        <s v="SAE 2015 BrainCloud video"/>
-        <s v="Tire Expo Booth"/>
-        <s v="Annual Report"/>
-        <s v="Misc"/>
-        <s v="UTC Web Site"/>
-        <s v="AVS One-Pagers"/>
-        <s v="Intranet"/>
-        <s v="VTTI Redesign"/>
-        <s v="Employee Directory"/>
-        <s v="VTTI Website"/>
-        <s v="NSTSCE Video"/>
-        <s v="LCD Panels"/>
-        <s v="ICMPA9 2015"/>
-        <s v="Motocycle Summit 2015"/>
-        <s v="MCOP Adaptive Lighting Project"/>
         <m/>
-        <s v="CAAR Web Site" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Sub-Task" numFmtId="0">
-      <sharedItems containsBlank="1" count="25">
+      <sharedItems containsBlank="1" count="5">
         <s v="RFP Submission"/>
+        <s v="Update"/>
         <s v="Conference Planning"/>
-        <s v="Set up &amp; Instruction"/>
-        <s v="Large Graphic Edit"/>
-        <s v="Medium graphic creation"/>
-        <s v="Animation"/>
-        <s v="Large graphic creation"/>
-        <s v="Small Graphic Edit"/>
-        <s v="Photography"/>
-        <s v="Update"/>
-        <s v="Creation"/>
-        <s v="Dealing with Ensemble"/>
-        <s v="File Clean-up"/>
-        <s v="Printing"/>
-        <s v="Filming"/>
-        <s v="Communication"/>
-        <s v="Training"/>
-        <s v="Answering Questions"/>
-        <s v="Demo Site"/>
-        <s v="Hardware"/>
-        <s v="Editing Content"/>
-        <s v="Creating Content"/>
-        <s v="Writing Content"/>
+        <s v="Invitations"/>
         <m/>
-        <s v="Invitations" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Month" numFmtId="0">
@@ -624,15 +582,15 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2014"/>
     </cacheField>
     <cacheField name="Hours" numFmtId="2">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="8"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="Person" numFmtId="0">
       <sharedItems containsBlank="1" count="6">
         <s v="Rodd"/>
+        <s v="April"/>
         <s v="Ceci"/>
         <s v="Marin"/>
         <s v="Justin"/>
-        <s v="April"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -646,7 +604,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="36">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -657,11 +615,19 @@
   </r>
   <r>
     <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -669,11 +635,19 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="4"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
+    <x v="0"/>
+    <n v="2014"/>
+    <n v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
@@ -685,7 +659,7 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -693,243 +667,19 @@
     <x v="0"/>
     <n v="2014"/>
     <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.25"/>
-    <x v="3"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2014"/>
-    <n v="0.5"/>
-    <x v="3"/>
+    <n v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="4"/>
     <x v="4"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.75"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="5"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="6"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="6.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="7"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.25"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="8"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.75"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="10"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="10"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="6"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="11"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="9"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="12"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="13"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="3.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="14"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="14"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="15"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="2"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="15"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="16"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="17"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="0"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="19"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="0.5"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="20"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <x v="21"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="4"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="22"/>
-    <x v="1"/>
-    <n v="2014"/>
-    <n v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="23"/>
     <x v="2"/>
     <m/>
     <m/>
@@ -939,68 +689,32 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item m="1" x="20"/>
+      <items count="6">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="19"/>
-        <item x="2"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="26">
-        <item x="1"/>
-        <item m="1" x="24"/>
-        <item x="0"/>
-        <item x="9"/>
-        <item x="23"/>
+      <items count="6">
         <item x="2"/>
         <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item h="1" x="2"/>
         <item t="default"/>
@@ -1010,10 +724,10 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="7">
+        <item x="1"/>
+        <item x="2"/>
         <item x="4"/>
-        <item x="1"/>
         <item x="3"/>
-        <item x="2"/>
         <item x="0"/>
         <item x="5"/>
         <item t="default"/>
@@ -1024,132 +738,33 @@
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="43">
+  <rowItems count="10">
     <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="10"/>
+      <x/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="1"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="12"/>
+      <x v="2"/>
     </i>
     <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1166,10 +781,10 @@
     <dataField name="Sum of Hours" fld="4" baseField="0" baseItem="1566352" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -1190,7 +805,7 @@
     <tableColumn id="2" name="Sub-Task"/>
     <tableColumn id="6" name="Month"/>
     <tableColumn id="7" name="Year"/>
-    <tableColumn id="4" name="Hours" dataDxfId="6"/>
+    <tableColumn id="4" name="Hours" dataDxfId="2"/>
     <tableColumn id="5" name="Person"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1462,9 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,10 +1100,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1499,13 +1114,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -1514,18 +1129,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>2014</v>
@@ -1534,18 +1149,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>2014</v>
@@ -1554,18 +1169,18 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>2014</v>
@@ -1574,18 +1189,18 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>2014</v>
@@ -1594,18 +1209,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -1614,18 +1229,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>2014</v>
@@ -1634,18 +1249,18 @@
         <v>1.25</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>2014</v>
@@ -1654,18 +1269,18 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>2014</v>
@@ -1674,18 +1289,18 @@
         <v>1.75</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>2014</v>
@@ -1694,18 +1309,18 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>2014</v>
@@ -1714,18 +1329,18 @@
         <v>6.5</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>2014</v>
@@ -1734,18 +1349,18 @@
         <v>1.25</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1754,18 +1369,18 @@
         <v>0.75</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1774,18 +1389,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>2014</v>
@@ -1794,18 +1409,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>2014</v>
@@ -1814,18 +1429,18 @@
         <v>4.5</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>2014</v>
@@ -1834,18 +1449,18 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>2014</v>
@@ -1854,18 +1469,18 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>2014</v>
@@ -1874,18 +1489,18 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>2014</v>
@@ -1894,18 +1509,18 @@
         <v>1.5</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>2014</v>
@@ -1914,18 +1529,18 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>2014</v>
@@ -1934,18 +1549,18 @@
         <v>3.5</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24">
         <v>2014</v>
@@ -1954,18 +1569,18 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>2014</v>
@@ -1974,18 +1589,18 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>2014</v>
@@ -1994,18 +1609,18 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>2014</v>
@@ -2014,18 +1629,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <v>2014</v>
@@ -2034,18 +1649,18 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>2014</v>
@@ -2054,18 +1669,18 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>2014</v>
@@ -2074,18 +1689,18 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>2014</v>
@@ -2094,18 +1709,18 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>2014</v>
@@ -2114,18 +1729,18 @@
         <v>0.5</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>2014</v>
@@ -2134,18 +1749,18 @@
         <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>2014</v>
@@ -2154,18 +1769,18 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>2014</v>
@@ -2174,18 +1789,18 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D36">
         <v>2014</v>
@@ -2194,7 +1809,7 @@
         <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2252,24 +1867,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,378 +1892,102 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>1.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
-        <v>1.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
-        <v>4.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4">
-        <v>1.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
-        <v>1.25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1.25</v>
-      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="4">
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="4">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="4">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="4">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53"/>
+      <c r="B16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2680,212 +2019,212 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2915,208 +2254,208 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
         <v>103</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +2480,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1">
         <v>2014</v>
@@ -3152,10 +2491,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>2015</v>
@@ -3163,10 +2502,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>2016</v>
@@ -3174,10 +2513,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2017</v>
@@ -3185,10 +2524,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -3196,10 +2535,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>2019</v>
@@ -3207,7 +2546,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2020</v>
@@ -3215,7 +2554,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -3223,7 +2562,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>2022</v>
@@ -3231,7 +2570,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>2023</v>
@@ -3239,12 +2578,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>